<commit_message>
Broke out intermediate calcualtions
</commit_message>
<xml_diff>
--- a/CH-129 Stocks.xlsx
+++ b/CH-129 Stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBB5782-923F-474A-B53C-47247F3E6D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E636D1C9-3E5A-42B0-A68F-9EFBD0016E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>Question</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>Acts as OR function</t>
   </si>
 </sst>
 </file>
@@ -2172,10 +2175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AA489A-7E53-4B71-958D-3E43FFA37807}">
-  <dimension ref="A1:O50"/>
+  <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2187,6 +2190,7 @@
     <col min="6" max="6" width="19.88671875" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2460,7 +2464,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="26">
         <v>45306</v>
@@ -2471,7 +2475,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="26">
         <v>45307</v>
@@ -2482,7 +2486,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="26">
         <v>45308</v>
@@ -2493,7 +2497,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="26">
         <v>45309</v>
@@ -2504,7 +2508,7 @@
       <c r="D20" s="9"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="26">
         <v>45310</v>
@@ -2515,7 +2519,7 @@
       <c r="D21" s="9"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="18">
         <v>45311</v>
@@ -2527,7 +2531,7 @@
       <c r="E22" s="1"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="18">
         <v>45312</v>
@@ -2538,7 +2542,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B24" s="18">
         <v>45313</v>
       </c>
@@ -2548,7 +2552,7 @@
       <c r="D24" s="9"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B25" s="18">
         <v>45314</v>
       </c>
@@ -2558,7 +2562,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B26" s="22">
         <v>45315</v>
       </c>
@@ -2572,8 +2576,11 @@
       <c r="H26" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J26" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G27" s="5" cm="1">
         <f t="array" ref="G27:G50">_xlfn.LET(
     _xlpm.b, B3:B26,
@@ -2602,8 +2609,24 @@
         <f t="array" ref="L27:L50">(_c &lt; _e) - (_e &lt; _a)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N27" cm="1">
+        <f t="array" ref="N27:N50">IF(_xlfn.ANCHORARRAY(J27) = 2, _b)</f>
+        <v>45292</v>
+      </c>
+      <c r="O27" t="b" cm="1">
+        <f t="array" ref="O27:O50">IF(_xlfn.ANCHORARRAY(J27) &lt;&gt; 2, _b)</f>
+        <v>0</v>
+      </c>
+      <c r="P27" cm="1">
+        <f t="array" ref="P27:P41">FREQUENCY(_xlfn.ANCHORARRAY(N27),_xlfn.ANCHORARRAY(O27))</f>
+        <v>2</v>
+      </c>
+      <c r="R27" cm="1">
+        <f t="array" ref="R27:R36">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(N27),--_xlfn.ANCHORARRAY(N27)&gt;0)</f>
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="str" cm="1">
         <f t="array" ref="B28:D29">_xlfn.LET(
     _xlpm.b, B3:B26,
@@ -2642,8 +2665,20 @@
       <c r="L28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <v>45293</v>
+      </c>
+      <c r="O28" t="b">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>45293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="str">
         <v>Downward</v>
       </c>
@@ -2665,8 +2700,20 @@
       <c r="L29">
         <v>-1</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>45294</v>
+      </c>
+      <c r="P29">
+        <v>4</v>
+      </c>
+      <c r="R29">
+        <v>45296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G30" s="5">
         <v>99</v>
       </c>
@@ -2679,8 +2726,20 @@
       <c r="L30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>45295</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>45297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G31" s="5">
         <v>43</v>
       </c>
@@ -2693,8 +2752,20 @@
       <c r="L31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N31">
+        <v>45296</v>
+      </c>
+      <c r="O31" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>45298</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G32" s="5">
         <v>52</v>
       </c>
@@ -2707,8 +2778,20 @@
       <c r="L32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N32">
+        <v>45297</v>
+      </c>
+      <c r="O32" t="b">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="33" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G33" s="5">
         <v>65</v>
       </c>
@@ -2721,8 +2804,20 @@
       <c r="L33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N33">
+        <v>45298</v>
+      </c>
+      <c r="O33" t="b">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>45311</v>
+      </c>
+    </row>
+    <row r="34" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G34" s="5">
         <v>72</v>
       </c>
@@ -2735,8 +2830,20 @@
       <c r="L34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N34">
+        <v>45299</v>
+      </c>
+      <c r="O34" t="b">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>45312</v>
+      </c>
+    </row>
+    <row r="35" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G35" s="5">
         <v>110</v>
       </c>
@@ -2749,8 +2856,20 @@
       <c r="L35">
         <v>-1</v>
       </c>
-    </row>
-    <row r="36" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>45300</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>45313</v>
+      </c>
+    </row>
+    <row r="36" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G36" s="5">
         <v>106</v>
       </c>
@@ -2763,8 +2882,20 @@
       <c r="L36">
         <v>-1</v>
       </c>
-    </row>
-    <row r="37" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N36" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>45301</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="37" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G37" s="5">
         <v>105</v>
       </c>
@@ -2777,8 +2908,17 @@
       <c r="L37">
         <v>-1</v>
       </c>
-    </row>
-    <row r="38" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N37" t="b">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>45302</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G38" s="5">
         <v>103</v>
       </c>
@@ -2791,8 +2931,17 @@
       <c r="L38">
         <v>-1</v>
       </c>
-    </row>
-    <row r="39" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>45303</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G39" s="5">
         <v>100</v>
       </c>
@@ -2805,8 +2954,17 @@
       <c r="L39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N39" t="b">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>45304</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G40" s="5">
         <v>85</v>
       </c>
@@ -2819,8 +2977,17 @@
       <c r="L40">
         <v>-1</v>
       </c>
-    </row>
-    <row r="41" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N40" t="b">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>45305</v>
+      </c>
+      <c r="P40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G41" s="5">
         <v>90</v>
       </c>
@@ -2833,8 +3000,17 @@
       <c r="L41">
         <v>-1</v>
       </c>
-    </row>
-    <row r="42" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N41" t="b">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>45306</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G42" s="5">
         <v>80</v>
       </c>
@@ -2847,8 +3023,14 @@
       <c r="L42">
         <v>-1</v>
       </c>
-    </row>
-    <row r="43" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N42" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>45307</v>
+      </c>
+    </row>
+    <row r="43" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G43" s="5">
         <v>61</v>
       </c>
@@ -2861,8 +3043,14 @@
       <c r="L43">
         <v>-1</v>
       </c>
-    </row>
-    <row r="44" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N43" t="b">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="44" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G44" s="5">
         <v>60</v>
       </c>
@@ -2875,8 +3063,14 @@
       <c r="L44">
         <v>-1</v>
       </c>
-    </row>
-    <row r="45" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N44" t="b">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="45" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G45" s="5">
         <v>55</v>
       </c>
@@ -2889,8 +3083,14 @@
       <c r="L45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N45" t="b">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>45310</v>
+      </c>
+    </row>
+    <row r="46" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G46" s="5">
         <v>52</v>
       </c>
@@ -2903,8 +3103,14 @@
       <c r="L46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N46">
+        <v>45311</v>
+      </c>
+      <c r="O46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G47" s="5">
         <v>75</v>
       </c>
@@ -2917,8 +3123,14 @@
       <c r="L47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N47">
+        <v>45312</v>
+      </c>
+      <c r="O47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G48" s="5">
         <v>84</v>
       </c>
@@ -2931,8 +3143,14 @@
       <c r="L48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N48">
+        <v>45313</v>
+      </c>
+      <c r="O48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G49" s="5">
         <v>94</v>
       </c>
@@ -2945,8 +3163,14 @@
       <c r="L49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="N49">
+        <v>45314</v>
+      </c>
+      <c r="O49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G50" s="5">
         <v>102</v>
       </c>
@@ -2958,6 +3182,12 @@
       </c>
       <c r="L50">
         <v>-1</v>
+      </c>
+      <c r="N50" t="b">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>45315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished looking at increasing part
</commit_message>
<xml_diff>
--- a/CH-129 Stocks.xlsx
+++ b/CH-129 Stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E636D1C9-3E5A-42B0-A68F-9EFBD0016E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA01D9F-7A4E-44E2-8590-5C340364738D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2175,10 +2175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AA489A-7E53-4B71-958D-3E43FFA37807}">
-  <dimension ref="A1:R50"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2464,7 +2464,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="26">
         <v>45306</v>
@@ -2475,7 +2475,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="26">
         <v>45307</v>
@@ -2486,7 +2486,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="26">
         <v>45308</v>
@@ -2497,7 +2497,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="26">
         <v>45309</v>
@@ -2508,7 +2508,7 @@
       <c r="D20" s="9"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="26">
         <v>45310</v>
@@ -2519,7 +2519,7 @@
       <c r="D21" s="9"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="18">
         <v>45311</v>
@@ -2531,7 +2531,7 @@
       <c r="E22" s="1"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="18">
         <v>45312</v>
@@ -2542,7 +2542,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B24" s="18">
         <v>45313</v>
       </c>
@@ -2552,7 +2552,7 @@
       <c r="D24" s="9"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B25" s="18">
         <v>45314</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B26" s="22">
         <v>45315</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G27" s="5" cm="1">
         <f t="array" ref="G27:G50">_xlfn.LET(
     _xlpm.b, B3:B26,
@@ -2621,12 +2621,20 @@
         <f t="array" ref="P27:P41">FREQUENCY(_xlfn.ANCHORARRAY(N27),_xlfn.ANCHORARRAY(O27))</f>
         <v>2</v>
       </c>
-      <c r="R27" cm="1">
-        <f t="array" ref="R27:R36">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(N27),--_xlfn.ANCHORARRAY(N27)&gt;0)</f>
+      <c r="Q27" cm="1">
+        <f t="array" ref="Q27:Q29">1+_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(P27),_xlfn.ANCHORARRAY(P27)&gt;0)</f>
+        <v>3</v>
+      </c>
+      <c r="R27">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(Q27))</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="S27" cm="1">
+        <f t="array" ref="S27:S36">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(N27),--_xlfn.ANCHORARRAY(N27)&gt;0)</f>
         <v>45292</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="str" cm="1">
         <f t="array" ref="B28:D29">_xlfn.LET(
     _xlpm.b, B3:B26,
@@ -2674,11 +2682,14 @@
       <c r="P28">
         <v>0</v>
       </c>
-      <c r="R28">
+      <c r="Q28">
+        <v>5</v>
+      </c>
+      <c r="S28">
         <v>45293</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="str">
         <v>Downward</v>
       </c>
@@ -2709,11 +2720,14 @@
       <c r="P29">
         <v>4</v>
       </c>
-      <c r="R29">
+      <c r="Q29">
+        <v>5</v>
+      </c>
+      <c r="S29">
         <v>45296</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G30" s="5">
         <v>99</v>
       </c>
@@ -2735,11 +2749,11 @@
       <c r="P30">
         <v>0</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <v>45297</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G31" s="5">
         <v>43</v>
       </c>
@@ -2761,11 +2775,11 @@
       <c r="P31">
         <v>0</v>
       </c>
-      <c r="R31">
+      <c r="S31">
         <v>45298</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G32" s="5">
         <v>52</v>
       </c>
@@ -2787,11 +2801,11 @@
       <c r="P32">
         <v>0</v>
       </c>
-      <c r="R32">
+      <c r="S32">
         <v>45299</v>
       </c>
     </row>
-    <row r="33" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G33" s="5">
         <v>65</v>
       </c>
@@ -2813,11 +2827,11 @@
       <c r="P33">
         <v>0</v>
       </c>
-      <c r="R33">
+      <c r="S33">
         <v>45311</v>
       </c>
     </row>
-    <row r="34" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G34" s="5">
         <v>72</v>
       </c>
@@ -2839,11 +2853,11 @@
       <c r="P34">
         <v>0</v>
       </c>
-      <c r="R34">
+      <c r="S34">
         <v>45312</v>
       </c>
     </row>
-    <row r="35" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G35" s="5">
         <v>110</v>
       </c>
@@ -2865,11 +2879,11 @@
       <c r="P35">
         <v>0</v>
       </c>
-      <c r="R35">
+      <c r="S35">
         <v>45313</v>
       </c>
     </row>
-    <row r="36" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G36" s="5">
         <v>106</v>
       </c>
@@ -2891,11 +2905,11 @@
       <c r="P36">
         <v>0</v>
       </c>
-      <c r="R36">
+      <c r="S36">
         <v>45314</v>
       </c>
     </row>
-    <row r="37" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G37" s="5">
         <v>105</v>
       </c>
@@ -2918,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G38" s="5">
         <v>103</v>
       </c>
@@ -2941,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G39" s="5">
         <v>100</v>
       </c>
@@ -2964,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G40" s="5">
         <v>85</v>
       </c>
@@ -2987,7 +3001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G41" s="5">
         <v>90</v>
       </c>
@@ -3010,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G42" s="5">
         <v>80</v>
       </c>
@@ -3030,7 +3044,7 @@
         <v>45307</v>
       </c>
     </row>
-    <row r="43" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G43" s="5">
         <v>61</v>
       </c>
@@ -3050,7 +3064,7 @@
         <v>45308</v>
       </c>
     </row>
-    <row r="44" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G44" s="5">
         <v>60</v>
       </c>
@@ -3070,7 +3084,7 @@
         <v>45309</v>
       </c>
     </row>
-    <row r="45" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G45" s="5">
         <v>55</v>
       </c>
@@ -3090,7 +3104,7 @@
         <v>45310</v>
       </c>
     </row>
-    <row r="46" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G46" s="5">
         <v>52</v>
       </c>
@@ -3110,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G47" s="5">
         <v>75</v>
       </c>
@@ -3130,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G48" s="5">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Put in commentary on my status
</commit_message>
<xml_diff>
--- a/CH-129 Stocks.xlsx
+++ b/CH-129 Stocks.xlsx
@@ -8,23 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110ABB45-D7C5-4A52-A755-13F4775B91BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E86874B-4829-4E5A-9BAF-1E7FAE7BD99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt1-Decline" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_a" localSheetId="3">'Alt1-Decline'!$G$27:$G$50</definedName>
     <definedName name="_a">'Alt1'!$G$27:$G$50</definedName>
+    <definedName name="_b" localSheetId="3">'Alt1-Decline'!$B$3:$B$26</definedName>
     <definedName name="_b">'Alt1'!$B$3:$B$26</definedName>
+    <definedName name="_c" localSheetId="3">'Alt1-Decline'!$C$3:$C$26</definedName>
     <definedName name="_c">'Alt1'!$C$3:$C$26</definedName>
+    <definedName name="_e" localSheetId="3">'Alt1-Decline'!$H$27:$H$50</definedName>
     <definedName name="_e">'Alt1'!$H$27:$H$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt1-Decline'!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Alt1'!$A$1:$F$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Alt1-Decline'!$B$1:$F$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
   <si>
     <t>Question</t>
   </si>
@@ -109,6 +117,15 @@
   <si>
     <t>Acts as OR function</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
 </sst>
 </file>
 
@@ -146,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +203,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,6 +454,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -740,6 +766,179 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3001979</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>51829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="A screenshot of a computer program&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D60F3865-824C-FFAE-81E3-768E995929B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="211015" y="5732585"/>
+          <a:ext cx="6249272" cy="3867690"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>310661</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>99646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>469795</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>151475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="A screenshot of a computer program&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BA679E4-026D-4C4C-9C58-F9FFF7C09C4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10064261" y="5105400"/>
+          <a:ext cx="6249272" cy="3867690"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>41030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257908</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>17584</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F7DB71F-E637-7DB6-BFC5-A59DBD891CB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5990492" y="1049215"/>
+          <a:ext cx="3053862" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>Okay, I finally have the logic figured</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t> out. I have documented in my notebook (I had to write it out). I will paste the relative sections in to this workbook later.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Basis">
   <a:themeElements>
@@ -1027,16 +1226,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="33"/>
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36"/>
       <c r="E1"/>
-      <c r="G1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="G1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
@@ -1440,10 +1639,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="33"/>
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36"/>
       <c r="E1">
         <v>-10</v>
       </c>
@@ -1451,11 +1650,11 @@
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
-      <c r="K1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="K1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
       <c r="O1" s="7" t="s">
         <v>9</v>
       </c>
@@ -2175,35 +2374,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AA489A-7E53-4B71-958D-3E43FFA37807}">
-  <dimension ref="A1:S75"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="3" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="57.21875" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="E1"/>
-      <c r="G1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="F1" s="7" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(F3)</f>
+        <v>=(_c&gt;_a)+(_e&gt;_a)</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
@@ -2215,8 +2419,12 @@
       <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2"/>
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
@@ -2234,8 +2442,17 @@
       <c r="C3" s="15">
         <v>47</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3"/>
+      <c r="D3" s="33">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E26" si="0">C4</f>
+        <v>62</v>
+      </c>
+      <c r="F3" s="2" cm="1">
+        <f t="array" ref="F3:F26">(_c&gt;_a)+(_e&gt;_a)</f>
+        <v>2</v>
+      </c>
       <c r="G3" s="12" t="s">
         <v>5</v>
       </c>
@@ -2259,8 +2476,17 @@
       <c r="C4" s="15">
         <v>62</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4"/>
+      <c r="D4" s="34">
+        <f t="shared" ref="D4:D26" si="1">C3</f>
+        <v>47</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
       <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
@@ -2283,8 +2509,17 @@
       <c r="C5" s="15">
         <v>99</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5"/>
+      <c r="D5" s="34">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
@@ -2301,8 +2536,17 @@
       <c r="C6" s="25">
         <v>43</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6"/>
+      <c r="D6" s="34">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
@@ -2319,8 +2563,17 @@
       <c r="C7" s="25">
         <v>52</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7"/>
+      <c r="D7" s="34">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -2333,9 +2586,17 @@
       <c r="C8" s="25">
         <v>65</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8"/>
+      <c r="D8" s="34">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
       <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
@@ -2352,9 +2613,17 @@
       <c r="C9" s="25">
         <v>72</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9"/>
+      <c r="D9" s="34">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9"/>
@@ -2371,9 +2640,17 @@
       <c r="C10" s="25">
         <v>110</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10"/>
+      <c r="D10" s="34">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10"/>
@@ -2390,9 +2667,17 @@
       <c r="C11" s="17">
         <v>106</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11"/>
+      <c r="D11" s="34">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11"/>
@@ -2409,9 +2694,17 @@
       <c r="C12" s="17">
         <v>105</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-      <c r="F12"/>
+      <c r="D12" s="34">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12"/>
@@ -2429,8 +2722,17 @@
       <c r="C13" s="17">
         <v>103</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="34">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="16">
@@ -2439,8 +2741,17 @@
       <c r="C14" s="17">
         <v>100</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
+      <c r="D14" s="34">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -2450,8 +2761,17 @@
       <c r="C15" s="17">
         <v>85</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
+      <c r="D15" s="34">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -2461,8 +2781,17 @@
       <c r="C16" s="27">
         <v>90</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="34">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -2472,8 +2801,17 @@
       <c r="C17" s="27">
         <v>80</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="34">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
@@ -2483,8 +2821,17 @@
       <c r="C18" s="27">
         <v>61</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="34">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -2494,8 +2841,17 @@
       <c r="C19" s="27">
         <v>60</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
+      <c r="D19" s="34">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
@@ -2505,8 +2861,17 @@
       <c r="C20" s="27">
         <v>55</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="34">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
@@ -2516,8 +2881,17 @@
       <c r="C21" s="27">
         <v>52</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="1"/>
+      <c r="D21" s="34">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
@@ -2527,8 +2901,17 @@
       <c r="C22" s="19">
         <v>75</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="34">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
@@ -2539,8 +2922,17 @@
       <c r="C23" s="19">
         <v>84</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="1"/>
+      <c r="D23" s="34">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B24" s="18">
@@ -2549,8 +2941,17 @@
       <c r="C24" s="19">
         <v>94</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="1"/>
+      <c r="D24" s="34">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B25" s="18">
@@ -2559,8 +2960,17 @@
       <c r="C25" s="19">
         <v>102</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="34">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B26" s="22">
@@ -2569,7 +2979,17 @@
       <c r="C26" s="23">
         <v>105</v>
       </c>
-      <c r="D26" s="9"/>
+      <c r="D26" s="34">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
       <c r="G26" s="5" t="s">
         <v>10</v>
       </c>
@@ -2581,6 +3001,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F27" s="2"/>
       <c r="G27" s="5" cm="1">
         <f t="array" ref="G27:G50">_xlfn.LET(
     _xlpm.b, B3:B26,
@@ -2657,6 +3078,7 @@
       <c r="D28">
         <v>5</v>
       </c>
+      <c r="F28" s="2"/>
       <c r="G28" s="5">
         <v>47</v>
       </c>
@@ -2696,6 +3118,7 @@
       <c r="D29">
         <v>6</v>
       </c>
+      <c r="F29" s="2"/>
       <c r="G29" s="5">
         <v>62</v>
       </c>
@@ -2722,6 +3145,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F30" s="2"/>
       <c r="G30" s="5">
         <v>99</v>
       </c>
@@ -2745,6 +3169,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F31" s="2"/>
       <c r="G31" s="5">
         <v>43</v>
       </c>
@@ -2768,6 +3193,7 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F32" s="2"/>
       <c r="G32" s="5">
         <v>52</v>
       </c>
@@ -2790,7 +3216,8 @@
         <v>45299</v>
       </c>
     </row>
-    <row r="33" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F33" s="2"/>
       <c r="G33" s="5">
         <v>65</v>
       </c>
@@ -2813,7 +3240,8 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="34" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F34" s="2"/>
       <c r="G34" s="5">
         <v>72</v>
       </c>
@@ -2836,7 +3264,8 @@
         <v>45312</v>
       </c>
     </row>
-    <row r="35" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F35" s="2"/>
       <c r="G35" s="5">
         <v>110</v>
       </c>
@@ -2859,7 +3288,8 @@
         <v>45313</v>
       </c>
     </row>
-    <row r="36" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F36" s="2"/>
       <c r="G36" s="5">
         <v>106</v>
       </c>
@@ -2882,7 +3312,8 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="37" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F37" s="2"/>
       <c r="G37" s="5">
         <v>105</v>
       </c>
@@ -2902,7 +3333,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F38" s="2"/>
       <c r="G38" s="5">
         <v>103</v>
       </c>
@@ -2922,7 +3354,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F39" s="2"/>
       <c r="G39" s="5">
         <v>100</v>
       </c>
@@ -2942,7 +3375,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F40" s="2"/>
       <c r="G40" s="5">
         <v>85</v>
       </c>
@@ -2962,7 +3396,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F41" s="2"/>
       <c r="G41" s="5">
         <v>90</v>
       </c>
@@ -2982,7 +3417,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F42" s="2"/>
       <c r="G42" s="5">
         <v>80</v>
       </c>
@@ -2999,7 +3435,8 @@
         <v>45307</v>
       </c>
     </row>
-    <row r="43" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F43" s="2"/>
       <c r="G43" s="5">
         <v>61</v>
       </c>
@@ -3016,7 +3453,8 @@
         <v>45308</v>
       </c>
     </row>
-    <row r="44" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F44" s="2"/>
       <c r="G44" s="5">
         <v>60</v>
       </c>
@@ -3033,7 +3471,8 @@
         <v>45309</v>
       </c>
     </row>
-    <row r="45" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F45" s="2"/>
       <c r="G45" s="5">
         <v>55</v>
       </c>
@@ -3050,7 +3489,8 @@
         <v>45310</v>
       </c>
     </row>
-    <row r="46" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F46" s="2"/>
       <c r="G46" s="5">
         <v>52</v>
       </c>
@@ -3067,7 +3507,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F47" s="2"/>
       <c r="G47" s="5">
         <v>75</v>
       </c>
@@ -3084,7 +3525,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F48" s="2"/>
       <c r="G48" s="5">
         <v>84</v>
       </c>
@@ -3101,7 +3543,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="F49" s="2"/>
       <c r="G49" s="5">
         <v>94</v>
       </c>
@@ -3118,7 +3561,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="F50" s="2"/>
       <c r="G50" s="5">
         <v>102</v>
       </c>
@@ -3135,7 +3579,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="52" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:19" x14ac:dyDescent="0.3">
       <c r="J52" cm="1">
         <f t="array" ref="J52:J75">(_c &lt; _e) - (_e &lt; _a)</f>
         <v>1</v>
@@ -3152,16 +3596,28 @@
         <f t="array" ref="P52:P65">FREQUENCY(_xlfn.ANCHORARRAY(N52),_xlfn.ANCHORARRAY(O52))</f>
         <v>0</v>
       </c>
-      <c r="Q52" cm="1">
-        <f t="array" ref="Q52:Q53">1+_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(P52),_xlfn.ANCHORARRAY(P52)&gt;1)</f>
+      <c r="R52" cm="1">
+        <f t="array" ref="R52:R53">1+_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(P52),_xlfn.ANCHORARRAY(P52)&gt;1)</f>
         <v>5</v>
       </c>
-      <c r="R52">
-        <f>AVERAGE(_xlfn.ANCHORARRAY(Q52))</f>
+      <c r="S52">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(R52))</f>
         <v>5.5</v>
       </c>
     </row>
-    <row r="53" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" s="5">
+        <v>1</v>
+      </c>
+      <c r="H53" s="5">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
       <c r="J53">
         <v>1</v>
       </c>
@@ -3174,15 +3630,39 @@
       <c r="P53">
         <v>0</v>
       </c>
-      <c r="Q53">
+      <c r="R53">
         <v>6</v>
       </c>
-      <c r="R53">
-        <f>MAX(_xlfn.ANCHORARRAY(Q52))</f>
+      <c r="S53">
+        <f>MAX(_xlfn.ANCHORARRAY(R52))</f>
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C54" cm="1">
+        <f t="array" ref="C54:C58">FREQUENCY(F53:F61,G53:G61)</f>
+        <v>0</v>
+      </c>
+      <c r="D54" cm="1">
+        <f t="array" ref="D54:D61">FREQUENCY(G53:G61,H53:H59)</f>
+        <v>0</v>
+      </c>
+      <c r="E54" cm="1">
+        <f t="array" ref="E54:E63">FREQUENCY(H53:H61,I53:I61)</f>
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" s="5">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
       <c r="J54">
         <v>-1</v>
       </c>
@@ -3196,7 +3676,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="5">
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
       <c r="J55">
         <v>0</v>
       </c>
@@ -3210,7 +3711,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" s="5">
+        <v>4</v>
+      </c>
+      <c r="H56" s="5">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
       <c r="J56">
         <v>1</v>
       </c>
@@ -3224,7 +3746,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" s="5">
+        <v>5</v>
+      </c>
+      <c r="H57" s="5">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
       <c r="J57">
         <v>1</v>
       </c>
@@ -3238,7 +3781,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>6</v>
+      </c>
+      <c r="G58" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" s="5">
+        <v>6</v>
+      </c>
+      <c r="I58">
+        <v>6</v>
+      </c>
       <c r="J58">
         <v>1</v>
       </c>
@@ -3252,7 +3816,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>7</v>
+      </c>
+      <c r="G59" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="5">
+        <v>7</v>
+      </c>
+      <c r="I59">
+        <v>7</v>
+      </c>
       <c r="J59">
         <v>0</v>
       </c>
@@ -3266,7 +3848,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="7:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>8</v>
+      </c>
+      <c r="G60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="5">
+        <v>8</v>
+      </c>
+      <c r="I60">
+        <v>8</v>
+      </c>
       <c r="J60">
         <v>-1</v>
       </c>
@@ -3279,8 +3879,34 @@
       <c r="P60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="7:18" x14ac:dyDescent="0.3">
+      <c r="R60" cm="1">
+        <f t="array" ref="R60:R73">FREQUENCY(_xlfn.ANCHORARRAY(N52),_xlfn.ANCHORARRAY(O52))</f>
+        <v>0</v>
+      </c>
+      <c r="S60" cm="1">
+        <f t="array" ref="S60:S61">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(R60),_xlfn.ANCHORARRAY(R60)&gt;1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" s="5">
+        <v>9</v>
+      </c>
+      <c r="H61" s="5">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
       <c r="J61">
         <v>-1</v>
       </c>
@@ -3293,8 +3919,17 @@
       <c r="P61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="7:18" x14ac:dyDescent="0.3">
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>0</v>
+      </c>
       <c r="J62">
         <v>-1</v>
       </c>
@@ -3307,8 +3942,14 @@
       <c r="P62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="7:18" x14ac:dyDescent="0.3">
+      <c r="R62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>0</v>
+      </c>
       <c r="J63">
         <v>-1</v>
       </c>
@@ -3321,8 +3962,11 @@
       <c r="P63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="7:18" x14ac:dyDescent="0.3">
+      <c r="R63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="3:19" x14ac:dyDescent="0.3">
       <c r="J64">
         <v>0</v>
       </c>
@@ -3335,8 +3979,15 @@
       <c r="P64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B65" s="4" cm="1">
+        <f t="array" ref="B65:B67">FREQUENCY({1,2,3,4,5}, {FALSE,2,4})</f>
+        <v>2</v>
+      </c>
       <c r="J65">
         <v>-1</v>
       </c>
@@ -3349,8 +4000,36 @@
       <c r="P65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B66" s="4">
+        <v>2</v>
+      </c>
+      <c r="D66" cm="1">
+        <f t="array" ref="D66:D71">FREQUENCY(E67:E74,I66:I70)</f>
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" cm="1">
+        <f t="array" ref="F66:F70">FREQUENCY(F53:F61,_xlfn._xlws.SORT(G53:G61))</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="5" cm="1">
+        <f t="array" ref="G66:G74">_xlfn._xlws.SORT(G53:G61)</f>
+        <v>1</v>
+      </c>
+      <c r="H66" s="5" cm="1">
+        <f t="array" ref="H66:H70">FREQUENCY(F53:F61,_xlfn.ANCHORARRAY(G66))</f>
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
       <c r="J66">
         <v>-1</v>
       </c>
@@ -3360,8 +4039,32 @@
       <c r="O66" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B67" s="4">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67" s="5">
+        <v>4</v>
+      </c>
+      <c r="H67" s="5">
+        <v>2</v>
+      </c>
+      <c r="I67">
+        <v>4</v>
+      </c>
       <c r="J67">
         <v>-1</v>
       </c>
@@ -3371,8 +4074,29 @@
       <c r="O67" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68" s="5">
+        <v>5</v>
+      </c>
+      <c r="H68" s="5">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>5</v>
+      </c>
       <c r="J68">
         <v>-1</v>
       </c>
@@ -3382,8 +4106,33 @@
       <c r="O68" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B69" s="4" cm="1">
+        <f t="array" ref="B69:B71">FREQUENCY({1,2,3,4,5}, {2,4})</f>
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>3</v>
+      </c>
+      <c r="G69" s="5">
+        <v>9</v>
+      </c>
+      <c r="H69" s="5">
+        <v>3</v>
+      </c>
+      <c r="I69">
+        <v>9</v>
+      </c>
       <c r="J69">
         <v>-1</v>
       </c>
@@ -3393,8 +4142,32 @@
       <c r="O69" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B70" s="4">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" s="5">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
       <c r="J70">
         <v>1</v>
       </c>
@@ -3404,8 +4177,23 @@
       <c r="O70">
         <v>45310</v>
       </c>
-    </row>
-    <row r="71" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B71" s="4">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>6</v>
+      </c>
+      <c r="G71" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J71">
         <v>1</v>
       </c>
@@ -3415,8 +4203,17 @@
       <c r="O71">
         <v>45311</v>
       </c>
-    </row>
-    <row r="72" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="E72">
+        <v>7</v>
+      </c>
+      <c r="G72" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J72">
         <v>1</v>
       </c>
@@ -3426,8 +4223,17 @@
       <c r="O72">
         <v>45312</v>
       </c>
-    </row>
-    <row r="73" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="E73">
+        <v>8</v>
+      </c>
+      <c r="G73" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J73">
         <v>1</v>
       </c>
@@ -3437,8 +4243,17 @@
       <c r="O73">
         <v>45313</v>
       </c>
-    </row>
-    <row r="74" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="R73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="E74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="J74">
         <v>1</v>
       </c>
@@ -3449,7 +4264,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="75" spans="10:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:18" x14ac:dyDescent="0.3">
       <c r="J75">
         <v>-1</v>
       </c>
@@ -3458,6 +4273,2424 @@
       </c>
       <c r="O75" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B77" s="4" cm="1">
+        <f t="array" ref="B77:B88">_xlfn._xlws.SORT(D77:D88)</f>
+        <v>0</v>
+      </c>
+      <c r="D77" s="1">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B78" s="4">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="F78" cm="1">
+        <f t="array" ref="F78:F88">_xlfn._xlws.SORT(D78:D88)</f>
+        <v>0</v>
+      </c>
+      <c r="N78" cm="1">
+        <f t="array" ref="N78:N88">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(N52),--_xlfn.ANCHORARRAY(N52)&gt;0)</f>
+        <v>45294</v>
+      </c>
+      <c r="P78">
+        <v>45292</v>
+      </c>
+      <c r="R78" cm="1">
+        <f t="array" ref="R78:R91">FREQUENCY(_xlfn.ANCHORARRAY(N78),P78:P90)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B79" s="4">
+        <v>2</v>
+      </c>
+      <c r="D79" s="32"/>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <v>45300</v>
+      </c>
+      <c r="P79">
+        <v>45293</v>
+      </c>
+      <c r="R79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B80" s="4">
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>2</v>
+      </c>
+      <c r="N80">
+        <v>45301</v>
+      </c>
+      <c r="P80">
+        <v>45295</v>
+      </c>
+      <c r="R80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B81" s="4">
+        <v>45292</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="F81">
+        <v>3</v>
+      </c>
+      <c r="N81">
+        <v>45302</v>
+      </c>
+      <c r="P81">
+        <v>45296</v>
+      </c>
+      <c r="R81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B82" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="F82" t="str">
+        <v>A</v>
+      </c>
+      <c r="N82">
+        <v>45303</v>
+      </c>
+      <c r="P82">
+        <v>45297</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B83" s="4" t="str">
+        <v>B</v>
+      </c>
+      <c r="D83" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" t="str">
+        <v>B</v>
+      </c>
+      <c r="N83">
+        <v>45305</v>
+      </c>
+      <c r="P83">
+        <v>45298</v>
+      </c>
+      <c r="R83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B84" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="D84" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" t="str">
+        <v>C</v>
+      </c>
+      <c r="N84">
+        <v>45306</v>
+      </c>
+      <c r="P84">
+        <v>45299</v>
+      </c>
+      <c r="R84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B85" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
+        <v>15</v>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N85">
+        <v>45307</v>
+      </c>
+      <c r="P85">
+        <v>45304</v>
+      </c>
+      <c r="R85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B86" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+      <c r="N86">
+        <v>45308</v>
+      </c>
+      <c r="P86">
+        <v>45310</v>
+      </c>
+      <c r="R86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B87" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D87" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N87">
+        <v>45309</v>
+      </c>
+      <c r="P87">
+        <v>45311</v>
+      </c>
+      <c r="R87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B88" s="4">
+        <v>0</v>
+      </c>
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="N88">
+        <v>45315</v>
+      </c>
+      <c r="P88">
+        <v>45312</v>
+      </c>
+      <c r="R88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P89">
+        <v>45313</v>
+      </c>
+      <c r="R89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P90">
+        <v>45314</v>
+      </c>
+      <c r="R90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="R91">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF1A046-F547-4362-B197-24FC19317B6C}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
+    <col min="3" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="F1" s="7" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(F3)</f>
+        <v>=-(_c&lt;_a)-(_e&lt;_a)</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="14">
+        <v>45292</v>
+      </c>
+      <c r="C3" s="15">
+        <v>47</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E26" si="0">C4</f>
+        <v>62</v>
+      </c>
+      <c r="F3" s="2" cm="1">
+        <f t="array" ref="F3:F26">-(_c&lt;_a)-(_e&lt;_a)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="29">
+        <f>AVERAGE(5,3,5)</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="I3" s="21">
+        <v>5</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="14">
+        <v>45293</v>
+      </c>
+      <c r="C4" s="15">
+        <v>62</v>
+      </c>
+      <c r="D4" s="34">
+        <f t="shared" ref="D4:D26" si="1">C3</f>
+        <v>47</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="29">
+        <v>5.5</v>
+      </c>
+      <c r="I4" s="21">
+        <v>6</v>
+      </c>
+      <c r="J4" s="13"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="14">
+        <v>45294</v>
+      </c>
+      <c r="C5" s="15">
+        <v>99</v>
+      </c>
+      <c r="D5" s="34">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="24">
+        <v>45295</v>
+      </c>
+      <c r="C6" s="25">
+        <v>43</v>
+      </c>
+      <c r="D6" s="34">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F6" s="2">
+        <v>-2</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="24">
+        <v>45296</v>
+      </c>
+      <c r="C7" s="25">
+        <v>52</v>
+      </c>
+      <c r="D7" s="34">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="24">
+        <v>45297</v>
+      </c>
+      <c r="C8" s="25">
+        <v>65</v>
+      </c>
+      <c r="D8" s="34">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="24">
+        <v>45298</v>
+      </c>
+      <c r="C9" s="25">
+        <v>72</v>
+      </c>
+      <c r="D9" s="34">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="24">
+        <v>45299</v>
+      </c>
+      <c r="C10" s="25">
+        <v>110</v>
+      </c>
+      <c r="D10" s="34">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+    </row>
+    <row r="11" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <v>45300</v>
+      </c>
+      <c r="C11" s="17">
+        <v>106</v>
+      </c>
+      <c r="D11" s="34">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="F11" s="2">
+        <v>-2</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+    </row>
+    <row r="12" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="16">
+        <v>45301</v>
+      </c>
+      <c r="C12" s="17">
+        <v>105</v>
+      </c>
+      <c r="D12" s="34">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="F12" s="2">
+        <v>-2</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="16">
+        <v>45302</v>
+      </c>
+      <c r="C13" s="17">
+        <v>103</v>
+      </c>
+      <c r="D13" s="34">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="16">
+        <v>45303</v>
+      </c>
+      <c r="C14" s="17">
+        <v>100</v>
+      </c>
+      <c r="D14" s="34">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="16">
+        <v>45304</v>
+      </c>
+      <c r="C15" s="17">
+        <v>85</v>
+      </c>
+      <c r="D15" s="34">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="26">
+        <v>45305</v>
+      </c>
+      <c r="C16" s="27">
+        <v>90</v>
+      </c>
+      <c r="D16" s="34">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="26">
+        <v>45306</v>
+      </c>
+      <c r="C17" s="27">
+        <v>80</v>
+      </c>
+      <c r="D17" s="34">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="26">
+        <v>45307</v>
+      </c>
+      <c r="C18" s="27">
+        <v>61</v>
+      </c>
+      <c r="D18" s="34">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="26">
+        <v>45308</v>
+      </c>
+      <c r="C19" s="27">
+        <v>60</v>
+      </c>
+      <c r="D19" s="34">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="26">
+        <v>45309</v>
+      </c>
+      <c r="C20" s="27">
+        <v>55</v>
+      </c>
+      <c r="D20" s="34">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="26">
+        <v>45310</v>
+      </c>
+      <c r="C21" s="27">
+        <v>52</v>
+      </c>
+      <c r="D21" s="34">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F21" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="18">
+        <v>45311</v>
+      </c>
+      <c r="C22" s="19">
+        <v>75</v>
+      </c>
+      <c r="D22" s="34">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="18">
+        <v>45312</v>
+      </c>
+      <c r="C23" s="19">
+        <v>84</v>
+      </c>
+      <c r="D23" s="34">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B24" s="18">
+        <v>45313</v>
+      </c>
+      <c r="C24" s="19">
+        <v>94</v>
+      </c>
+      <c r="D24" s="34">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B25" s="18">
+        <v>45314</v>
+      </c>
+      <c r="C25" s="19">
+        <v>102</v>
+      </c>
+      <c r="D25" s="34">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B26" s="22">
+        <v>45315</v>
+      </c>
+      <c r="C26" s="23">
+        <v>105</v>
+      </c>
+      <c r="D26" s="34">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F27" s="2"/>
+      <c r="G27" s="5" cm="1">
+        <f t="array" ref="G27:G50">_xlfn.LET(
+    _xlpm.b, B3:B26,
+    _xlpm.c, C3:C26,
+    _xlpm.a, _xlfn.VSTACK(0, _xlfn.DROP(_xlpm.c, -1)),
+    _xlpm.e, _xlfn.VSTACK(_xlfn.DROP(_xlpm.c, 1), 0),
+   _xlpm.a
+)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="5" cm="1">
+        <f t="array" ref="H27:H50">_xlfn.LET(
+    _xlpm.b, B3:B26,
+    _xlpm.c, C3:C26,
+    _xlpm.a, _xlfn.VSTACK(0, _xlfn.DROP(_xlpm.c, -1)),
+    _xlpm.e, _xlfn.VSTACK(_xlfn.DROP(_xlpm.c, 1), 0),
+   _xlpm.e
+)</f>
+        <v>62</v>
+      </c>
+      <c r="J27" cm="1">
+        <f t="array" ref="J27:J50">(_c &gt; _a) + (_e &gt; _a)</f>
+        <v>2</v>
+      </c>
+      <c r="N27" cm="1">
+        <f t="array" ref="N27:N50">IF(_xlfn.ANCHORARRAY(J27) = 2, _b)</f>
+        <v>45292</v>
+      </c>
+      <c r="O27" t="b" cm="1">
+        <f t="array" ref="O27:O50">IF(_xlfn.ANCHORARRAY(J27) &lt;&gt; 2, _b)</f>
+        <v>0</v>
+      </c>
+      <c r="P27" cm="1">
+        <f t="array" ref="P27:P41">FREQUENCY(_xlfn.ANCHORARRAY(N27),_xlfn.ANCHORARRAY(O27))</f>
+        <v>2</v>
+      </c>
+      <c r="Q27" cm="1">
+        <f t="array" ref="Q27:Q29">1+_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(P27),_xlfn.ANCHORARRAY(P27)&gt;1)</f>
+        <v>3</v>
+      </c>
+      <c r="R27">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(Q27))</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="S27" cm="1">
+        <f t="array" ref="S27:S36">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(N27),--_xlfn.ANCHORARRAY(N27)&gt;0)</f>
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="str" cm="1">
+        <f t="array" ref="B28:D29">_xlfn.LET(
+    _xlpm.b, B3:B26,
+    _xlpm.c, C3:C26,
+    _xlpm.a, _xlfn.VSTACK(0, _xlfn.DROP(_xlpm.c, -1)),
+    _xlpm.e, _xlfn.VSTACK(_xlfn.DROP(_xlpm.c, 1), 0),
+    _xlpm.F, _xlfn.LAMBDA(_xlpm.i,_xlpm.j,
+        _xlfn.LET(
+            _xlpm.f, FREQUENCY(IF(_xlpm.i = _xlpm.j, _xlpm.b), IF(_xlpm.i &lt;&gt; _xlpm.j, _xlpm.b)),
+            _xlpm.g, 1 + _xlfn._xlws.FILTER(_xlpm.f, _xlpm.f &gt; 1),
+            _xlfn.HSTACK(AVERAGE(_xlpm.g), MAX(_xlpm.g))
+        )
+    ),
+    _xlfn.HSTACK(
+        {"Up";"Down"} &amp; "ward",
+        _xlfn.VSTACK(_xlpm.F((_xlpm.c &gt; _xlpm.a) + (_xlpm.e &gt; _xlpm.a), 2), _xlpm.F(-(_xlpm.c &lt; _xlpm.a) - (_xlpm.e &lt; _xlpm.a), -2))
+    )
+)</f>
+        <v>Upward</v>
+      </c>
+      <c r="C28">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="5">
+        <v>47</v>
+      </c>
+      <c r="H28" s="5">
+        <v>99</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <v>45293</v>
+      </c>
+      <c r="O28" t="b">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>5</v>
+      </c>
+      <c r="R28">
+        <f>MAX(_xlfn.ANCHORARRAY(Q27))</f>
+        <v>5</v>
+      </c>
+      <c r="S28">
+        <v>45293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B29" s="4" t="str">
+        <v>Downward</v>
+      </c>
+      <c r="C29">
+        <v>5.5</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="5">
+        <v>62</v>
+      </c>
+      <c r="H29" s="5">
+        <v>43</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="N29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>45294</v>
+      </c>
+      <c r="P29">
+        <v>4</v>
+      </c>
+      <c r="Q29">
+        <v>5</v>
+      </c>
+      <c r="S29">
+        <v>45296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F30" s="2"/>
+      <c r="G30" s="5">
+        <v>99</v>
+      </c>
+      <c r="H30" s="5">
+        <v>52</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="N30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>45295</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>45297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F31" s="2"/>
+      <c r="G31" s="5">
+        <v>43</v>
+      </c>
+      <c r="H31" s="5">
+        <v>65</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="N31">
+        <v>45296</v>
+      </c>
+      <c r="O31" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>45298</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F32" s="2"/>
+      <c r="G32" s="5">
+        <v>52</v>
+      </c>
+      <c r="H32" s="5">
+        <v>72</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>45297</v>
+      </c>
+      <c r="O32" t="b">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="33" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F33" s="2"/>
+      <c r="G33" s="5">
+        <v>65</v>
+      </c>
+      <c r="H33" s="5">
+        <v>110</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="N33">
+        <v>45298</v>
+      </c>
+      <c r="O33" t="b">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>45311</v>
+      </c>
+    </row>
+    <row r="34" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F34" s="2"/>
+      <c r="G34" s="5">
+        <v>72</v>
+      </c>
+      <c r="H34" s="5">
+        <v>106</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="N34">
+        <v>45299</v>
+      </c>
+      <c r="O34" t="b">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>45312</v>
+      </c>
+    </row>
+    <row r="35" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F35" s="2"/>
+      <c r="G35" s="5">
+        <v>110</v>
+      </c>
+      <c r="H35" s="5">
+        <v>105</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="N35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>45300</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>45313</v>
+      </c>
+    </row>
+    <row r="36" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F36" s="2"/>
+      <c r="G36" s="5">
+        <v>106</v>
+      </c>
+      <c r="H36" s="5">
+        <v>103</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="N36" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>45301</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="37" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F37" s="2"/>
+      <c r="G37" s="5">
+        <v>105</v>
+      </c>
+      <c r="H37" s="5">
+        <v>100</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="N37" t="b">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>45302</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F38" s="2"/>
+      <c r="G38" s="5">
+        <v>103</v>
+      </c>
+      <c r="H38" s="5">
+        <v>85</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="N38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>45303</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F39" s="2"/>
+      <c r="G39" s="5">
+        <v>100</v>
+      </c>
+      <c r="H39" s="5">
+        <v>90</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="N39" t="b">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>45304</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F40" s="2"/>
+      <c r="G40" s="5">
+        <v>85</v>
+      </c>
+      <c r="H40" s="5">
+        <v>80</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="N40" t="b">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>45305</v>
+      </c>
+      <c r="P40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F41" s="2"/>
+      <c r="G41" s="5">
+        <v>90</v>
+      </c>
+      <c r="H41" s="5">
+        <v>61</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="N41" t="b">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>45306</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F42" s="2"/>
+      <c r="G42" s="5">
+        <v>80</v>
+      </c>
+      <c r="H42" s="5">
+        <v>60</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="N42" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>45307</v>
+      </c>
+    </row>
+    <row r="43" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F43" s="2"/>
+      <c r="G43" s="5">
+        <v>61</v>
+      </c>
+      <c r="H43" s="5">
+        <v>55</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="N43" t="b">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="44" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F44" s="2"/>
+      <c r="G44" s="5">
+        <v>60</v>
+      </c>
+      <c r="H44" s="5">
+        <v>52</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="N44" t="b">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="45" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F45" s="2"/>
+      <c r="G45" s="5">
+        <v>55</v>
+      </c>
+      <c r="H45" s="5">
+        <v>75</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="N45" t="b">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>45310</v>
+      </c>
+    </row>
+    <row r="46" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F46" s="2"/>
+      <c r="G46" s="5">
+        <v>52</v>
+      </c>
+      <c r="H46" s="5">
+        <v>84</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="N46">
+        <v>45311</v>
+      </c>
+      <c r="O46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F47" s="2"/>
+      <c r="G47" s="5">
+        <v>75</v>
+      </c>
+      <c r="H47" s="5">
+        <v>94</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="N47">
+        <v>45312</v>
+      </c>
+      <c r="O47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F48" s="2"/>
+      <c r="G48" s="5">
+        <v>84</v>
+      </c>
+      <c r="H48" s="5">
+        <v>102</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="N48">
+        <v>45313</v>
+      </c>
+      <c r="O48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="F49" s="2"/>
+      <c r="G49" s="5">
+        <v>94</v>
+      </c>
+      <c r="H49" s="5">
+        <v>105</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="N49">
+        <v>45314</v>
+      </c>
+      <c r="O49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="F50" s="2"/>
+      <c r="G50" s="5">
+        <v>102</v>
+      </c>
+      <c r="H50" s="5">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="N50" t="b">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="52" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="J52" cm="1">
+        <f t="array" ref="J52:J75">(_c &lt; _e) - (_e &lt; _a)</f>
+        <v>1</v>
+      </c>
+      <c r="N52" t="b" cm="1">
+        <f t="array" ref="N52:N75">IF(_xlfn.ANCHORARRAY(J52) = -1, _b)</f>
+        <v>0</v>
+      </c>
+      <c r="O52" cm="1">
+        <f t="array" ref="O52:O75">IF(_xlfn.ANCHORARRAY(J52) &lt;&gt; -1, _b)</f>
+        <v>45292</v>
+      </c>
+      <c r="P52" cm="1">
+        <f t="array" ref="P52:P65">FREQUENCY(_xlfn.ANCHORARRAY(N52),_xlfn.ANCHORARRAY(O52))</f>
+        <v>0</v>
+      </c>
+      <c r="R52" cm="1">
+        <f t="array" ref="R52:R53">1+_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(P52),_xlfn.ANCHORARRAY(P52)&gt;1)</f>
+        <v>5</v>
+      </c>
+      <c r="S52">
+        <f>AVERAGE(_xlfn.ANCHORARRAY(R52))</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="53" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" s="5">
+        <v>1</v>
+      </c>
+      <c r="H53" s="5">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="N53" t="b">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>45293</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>6</v>
+      </c>
+      <c r="S53">
+        <f>MAX(_xlfn.ANCHORARRAY(R52))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C54" cm="1">
+        <f t="array" ref="C54:C58">FREQUENCY(F53:F61,G53:G61)</f>
+        <v>0</v>
+      </c>
+      <c r="D54" cm="1">
+        <f t="array" ref="D54:D61">FREQUENCY(G53:G61,H53:H59)</f>
+        <v>0</v>
+      </c>
+      <c r="E54" cm="1">
+        <f t="array" ref="E54:E63">FREQUENCY(H53:H61,I53:I61)</f>
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" s="5">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="J54">
+        <v>-1</v>
+      </c>
+      <c r="N54">
+        <v>45294</v>
+      </c>
+      <c r="O54" t="b">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="5">
+        <v>3</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="N55" t="b">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>45295</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" s="5">
+        <v>4</v>
+      </c>
+      <c r="H56" s="5">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="N56" t="b">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>45296</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" s="5">
+        <v>5</v>
+      </c>
+      <c r="H57" s="5">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="N57" t="b">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>45297</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>6</v>
+      </c>
+      <c r="G58" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" s="5">
+        <v>6</v>
+      </c>
+      <c r="I58">
+        <v>6</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="N58" t="b">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>45298</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>7</v>
+      </c>
+      <c r="G59" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="5">
+        <v>7</v>
+      </c>
+      <c r="I59">
+        <v>7</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="N59" t="b">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>45299</v>
+      </c>
+      <c r="P59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>8</v>
+      </c>
+      <c r="G60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="5">
+        <v>8</v>
+      </c>
+      <c r="I60">
+        <v>8</v>
+      </c>
+      <c r="J60">
+        <v>-1</v>
+      </c>
+      <c r="N60">
+        <v>45300</v>
+      </c>
+      <c r="O60" t="b">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>5</v>
+      </c>
+      <c r="R60" cm="1">
+        <f t="array" ref="R60:R73">FREQUENCY(_xlfn.ANCHORARRAY(N52),_xlfn.ANCHORARRAY(O52))</f>
+        <v>0</v>
+      </c>
+      <c r="S60" cm="1">
+        <f t="array" ref="S60:S61">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(R60),_xlfn.ANCHORARRAY(R60)&gt;1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" s="5">
+        <v>9</v>
+      </c>
+      <c r="H61" s="5">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>-1</v>
+      </c>
+      <c r="N61">
+        <v>45301</v>
+      </c>
+      <c r="O61" t="b">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>-1</v>
+      </c>
+      <c r="N62">
+        <v>45302</v>
+      </c>
+      <c r="O62" t="b">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>-1</v>
+      </c>
+      <c r="N63">
+        <v>45303</v>
+      </c>
+      <c r="O63" t="b">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="N64" t="b">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>45304</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B65" s="4" cm="1">
+        <f t="array" ref="B65:B67">FREQUENCY({1,2,3,4,5}, {FALSE,2,4})</f>
+        <v>2</v>
+      </c>
+      <c r="J65">
+        <v>-1</v>
+      </c>
+      <c r="N65">
+        <v>45305</v>
+      </c>
+      <c r="O65" t="b">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>1</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B66" s="4">
+        <v>2</v>
+      </c>
+      <c r="D66" cm="1">
+        <f t="array" ref="D66:D71">FREQUENCY(E67:E74,I66:I70)</f>
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" cm="1">
+        <f t="array" ref="F66:F70">FREQUENCY(F53:F61,_xlfn._xlws.SORT(G53:G61))</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="5" cm="1">
+        <f t="array" ref="G66:G74">_xlfn._xlws.SORT(G53:G61)</f>
+        <v>1</v>
+      </c>
+      <c r="H66" s="5" cm="1">
+        <f t="array" ref="H66:H70">FREQUENCY(F53:F61,_xlfn.ANCHORARRAY(G66))</f>
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>-1</v>
+      </c>
+      <c r="N66">
+        <v>45306</v>
+      </c>
+      <c r="O66" t="b">
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B67" s="4">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67" s="5">
+        <v>4</v>
+      </c>
+      <c r="H67" s="5">
+        <v>2</v>
+      </c>
+      <c r="I67">
+        <v>4</v>
+      </c>
+      <c r="J67">
+        <v>-1</v>
+      </c>
+      <c r="N67">
+        <v>45307</v>
+      </c>
+      <c r="O67" t="b">
+        <v>0</v>
+      </c>
+      <c r="R67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68" s="5">
+        <v>5</v>
+      </c>
+      <c r="H68" s="5">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>5</v>
+      </c>
+      <c r="J68">
+        <v>-1</v>
+      </c>
+      <c r="N68">
+        <v>45308</v>
+      </c>
+      <c r="O68" t="b">
+        <v>0</v>
+      </c>
+      <c r="R68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B69" s="4" cm="1">
+        <f t="array" ref="B69:B71">FREQUENCY({1,2,3,4,5}, {2,4})</f>
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>3</v>
+      </c>
+      <c r="G69" s="5">
+        <v>9</v>
+      </c>
+      <c r="H69" s="5">
+        <v>3</v>
+      </c>
+      <c r="I69">
+        <v>9</v>
+      </c>
+      <c r="J69">
+        <v>-1</v>
+      </c>
+      <c r="N69">
+        <v>45309</v>
+      </c>
+      <c r="O69" t="b">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B70" s="4">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" s="5">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="N70" t="b">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>45310</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B71" s="4">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>6</v>
+      </c>
+      <c r="G71" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="N71" t="b">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>45311</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="E72">
+        <v>7</v>
+      </c>
+      <c r="G72" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="N72" t="b">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>45312</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="E73">
+        <v>8</v>
+      </c>
+      <c r="G73" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="N73" t="b">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>45313</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="E74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="N74" t="b">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J75">
+        <v>-1</v>
+      </c>
+      <c r="N75">
+        <v>45315</v>
+      </c>
+      <c r="O75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B77" s="4" cm="1">
+        <f t="array" ref="B77:B88">_xlfn._xlws.SORT(D77:D88)</f>
+        <v>0</v>
+      </c>
+      <c r="D77" s="1">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B78" s="4">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="F78" cm="1">
+        <f t="array" ref="F78:F88">_xlfn._xlws.SORT(D78:D88)</f>
+        <v>0</v>
+      </c>
+      <c r="N78" cm="1">
+        <f t="array" ref="N78:N88">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(N52),--_xlfn.ANCHORARRAY(N52)&gt;0)</f>
+        <v>45294</v>
+      </c>
+      <c r="P78">
+        <v>45292</v>
+      </c>
+      <c r="R78" cm="1">
+        <f t="array" ref="R78:R91">FREQUENCY(_xlfn.ANCHORARRAY(N78),P78:P90)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B79" s="4">
+        <v>2</v>
+      </c>
+      <c r="D79" s="32"/>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <v>45300</v>
+      </c>
+      <c r="P79">
+        <v>45293</v>
+      </c>
+      <c r="R79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B80" s="4">
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>2</v>
+      </c>
+      <c r="N80">
+        <v>45301</v>
+      </c>
+      <c r="P80">
+        <v>45295</v>
+      </c>
+      <c r="R80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B81" s="4">
+        <v>45292</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="F81">
+        <v>3</v>
+      </c>
+      <c r="N81">
+        <v>45302</v>
+      </c>
+      <c r="P81">
+        <v>45296</v>
+      </c>
+      <c r="R81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B82" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="F82" t="str">
+        <v>A</v>
+      </c>
+      <c r="N82">
+        <v>45303</v>
+      </c>
+      <c r="P82">
+        <v>45297</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B83" s="4" t="str">
+        <v>B</v>
+      </c>
+      <c r="D83" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" t="str">
+        <v>B</v>
+      </c>
+      <c r="N83">
+        <v>45305</v>
+      </c>
+      <c r="P83">
+        <v>45298</v>
+      </c>
+      <c r="R83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B84" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="D84" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" t="str">
+        <v>C</v>
+      </c>
+      <c r="N84">
+        <v>45306</v>
+      </c>
+      <c r="P84">
+        <v>45299</v>
+      </c>
+      <c r="R84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B85" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
+        <v>15</v>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+      <c r="N85">
+        <v>45307</v>
+      </c>
+      <c r="P85">
+        <v>45304</v>
+      </c>
+      <c r="R85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B86" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+      <c r="N86">
+        <v>45308</v>
+      </c>
+      <c r="P86">
+        <v>45310</v>
+      </c>
+      <c r="R86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B87" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D87" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N87">
+        <v>45309</v>
+      </c>
+      <c r="P87">
+        <v>45311</v>
+      </c>
+      <c r="R87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B88" s="4">
+        <v>0</v>
+      </c>
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="N88">
+        <v>45315</v>
+      </c>
+      <c r="P88">
+        <v>45312</v>
+      </c>
+      <c r="R88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P89">
+        <v>45313</v>
+      </c>
+      <c r="R89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P90">
+        <v>45314</v>
+      </c>
+      <c r="R90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="R91">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3467,5 +6700,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All done. Last work in notebook
</commit_message>
<xml_diff>
--- a/CH-129 Stocks.xlsx
+++ b/CH-129 Stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E86874B-4829-4E5A-9BAF-1E7FAE7BD99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49AB36F-15B7-4637-9B8E-4429649E80E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -936,6 +936,81 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>316523</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>169984</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>269631</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>146538</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF473FF9-5DA1-6D12-F1AE-415E97946E68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6002215" y="2268415"/>
+          <a:ext cx="3053862" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>I am now</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t> done with this drill. No more juice to squeeze. I have documented my work in the notebook.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4546,7 +4621,7 @@
   <dimension ref="A1:S91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>